<commit_message>
melhoria no sistema de alteração de dados
</commit_message>
<xml_diff>
--- a/Assets/Data/Template.xlsx
+++ b/Assets/Data/Template.xlsx
@@ -540,25 +540,31 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Victor</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>9384756</v>
-      </c>
-      <c r="C5" t="n">
-        <v>98475</v>
-      </c>
-      <c r="D5" t="n">
-        <v>7465</v>
+          <t>Victor Nascimento</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>934856</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>9487</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4987</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>victornjg@gmail.com</t>
+          <t>victornascimento@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>349847562</v>
+        <v>344557543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>